<commit_message>
Bring data up to date
</commit_message>
<xml_diff>
--- a/benchmarks/mc2022/total_X_definition.xlsx
+++ b/benchmarks/mc2022/total_X_definition.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bryant/repos/model-counting/benchmarks/mc2022/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{163F31FC-3BDD-7E47-B39E-C731C5C94E29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{762CDE76-ADCE-C344-840C-06A87D1E6C02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11920" yWindow="500" windowWidth="35140" windowHeight="26660" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="57840" yWindow="7380" windowWidth="35140" windowHeight="26660" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="v01-no-lemmas" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="128">
   <si>
     <t>Instance</t>
   </si>
@@ -274,21 +274,12 @@
     <t>mc2022_track2_053</t>
   </si>
   <si>
-    <t>mc2022_track2_085</t>
-  </si>
-  <si>
     <t>mc2022_track2_089</t>
   </si>
   <si>
-    <t>mc2022_track2_097</t>
-  </si>
-  <si>
     <t>mc2022_track2_101</t>
   </si>
   <si>
-    <t>mc2022_track2_107</t>
-  </si>
-  <si>
     <t>mc2022_track2_125</t>
   </si>
   <si>
@@ -338,12 +329,106 @@
   </si>
   <si>
     <t>mc2022_track2_035</t>
+  </si>
+  <si>
+    <t>mc2022_track1_049</t>
+  </si>
+  <si>
+    <t>mc2022_track1_069</t>
+  </si>
+  <si>
+    <t>mc2022_track1_071</t>
+  </si>
+  <si>
+    <t>mc2022_track1_083</t>
+  </si>
+  <si>
+    <t>mc2022_track1_089</t>
+  </si>
+  <si>
+    <t>mc2022_track1_099</t>
+  </si>
+  <si>
+    <t>mc2022_track1_107</t>
+  </si>
+  <si>
+    <t>mc2022_track1_117</t>
+  </si>
+  <si>
+    <t>mc2022_track1_121</t>
+  </si>
+  <si>
+    <t>mc2022_track1_125</t>
+  </si>
+  <si>
+    <t>mc2022_track1_127</t>
+  </si>
+  <si>
+    <t>mc2022_track1_133</t>
+  </si>
+  <si>
+    <t>mc2022_track1_135</t>
+  </si>
+  <si>
+    <t>mc2022_track1_145</t>
+  </si>
+  <si>
+    <t>mc2022_track1_157</t>
+  </si>
+  <si>
+    <t>mc2022_track1_167</t>
+  </si>
+  <si>
+    <t>mc2022_track2_001</t>
+  </si>
+  <si>
+    <t>mc2022_track2_055</t>
+  </si>
+  <si>
+    <t>mc2022_track2_061</t>
+  </si>
+  <si>
+    <t>mc2022_track2_079</t>
+  </si>
+  <si>
+    <t>mc2022_track2_091</t>
+  </si>
+  <si>
+    <t>mc2022_track2_111</t>
+  </si>
+  <si>
+    <t>mc2022_track2_139</t>
+  </si>
+  <si>
+    <t>mc2022_track2_179</t>
+  </si>
+  <si>
+    <t>mc2022_track2_181</t>
+  </si>
+  <si>
+    <t>mc2022_track2_199</t>
+  </si>
+  <si>
+    <t>Defining</t>
+  </si>
+  <si>
+    <t>min</t>
+  </si>
+  <si>
+    <t>max</t>
+  </si>
+  <si>
+    <t>mean</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="2">
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -777,7 +862,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -820,13 +905,15 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="42" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="42">
+  <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -854,6 +941,7 @@
     <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
     <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
     <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Comma" xfId="42" builtinId="3"/>
     <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
     <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
     <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
@@ -2528,70 +2616,70 @@
                   <c:v>3191</c:v>
                 </c:pt>
                 <c:pt idx="22">
+                  <c:v>5985623</c:v>
+                </c:pt>
+                <c:pt idx="23">
                   <c:v>467550</c:v>
                 </c:pt>
-                <c:pt idx="23">
+                <c:pt idx="24">
                   <c:v>1318024</c:v>
                 </c:pt>
-                <c:pt idx="24">
+                <c:pt idx="25">
                   <c:v>4713</c:v>
                 </c:pt>
-                <c:pt idx="25">
+                <c:pt idx="26">
                   <c:v>1682059</c:v>
                 </c:pt>
-                <c:pt idx="26">
+                <c:pt idx="27">
                   <c:v>1406192</c:v>
                 </c:pt>
-                <c:pt idx="27">
+                <c:pt idx="28">
                   <c:v>899701</c:v>
                 </c:pt>
-                <c:pt idx="28">
+                <c:pt idx="29">
+                  <c:v>4936014</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>8038928</c:v>
+                </c:pt>
+                <c:pt idx="31">
                   <c:v>70651620</c:v>
                 </c:pt>
-                <c:pt idx="29">
+                <c:pt idx="32">
                   <c:v>9567</c:v>
                 </c:pt>
-                <c:pt idx="30">
+                <c:pt idx="33">
                   <c:v>39501</c:v>
                 </c:pt>
-                <c:pt idx="31">
+                <c:pt idx="34">
                   <c:v>18007</c:v>
                 </c:pt>
-                <c:pt idx="32">
+                <c:pt idx="35">
+                  <c:v>125319627</c:v>
+                </c:pt>
+                <c:pt idx="36">
                   <c:v>82194</c:v>
                 </c:pt>
-                <c:pt idx="33">
+                <c:pt idx="37">
+                  <c:v>269645146</c:v>
+                </c:pt>
+                <c:pt idx="38">
                   <c:v>304</c:v>
                 </c:pt>
-                <c:pt idx="34">
+                <c:pt idx="39">
                   <c:v>574062</c:v>
                 </c:pt>
-                <c:pt idx="35">
+                <c:pt idx="40">
                   <c:v>887</c:v>
                 </c:pt>
-                <c:pt idx="36">
+                <c:pt idx="41">
                   <c:v>1757</c:v>
                 </c:pt>
-                <c:pt idx="37">
+                <c:pt idx="42">
+                  <c:v>78873354</c:v>
+                </c:pt>
+                <c:pt idx="43">
                   <c:v>190248</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>2064844</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>50722</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>45923418</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>72258</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>401032</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>355</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2606,19 +2694,19 @@
                   <c:v>161794</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2392</c:v>
+                  <c:v>2397</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>4427</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>262327</c:v>
+                  <c:v>262373</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>6077</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>549</c:v>
+                  <c:v>554</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>14373</c:v>
@@ -2627,19 +2715,19 @@
                   <c:v>1213826</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>81776</c:v>
+                  <c:v>81780</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>33206</c:v>
+                  <c:v>33207</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1117366</c:v>
+                  <c:v>1117440</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>3809317</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>2211854</c:v>
+                  <c:v>2211944</c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>2393131</c:v>
@@ -2651,7 +2739,7 @@
                   <c:v>13207</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>721933</c:v>
+                  <c:v>721935</c:v>
                 </c:pt>
                 <c:pt idx="17">
                   <c:v>13101</c:v>
@@ -2663,76 +2751,76 @@
                   <c:v>46079</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>1593572</c:v>
+                  <c:v>1593947</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>26361</c:v>
+                  <c:v>26378</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>940813</c:v>
+                  <c:v>28392373</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>2813556</c:v>
+                  <c:v>940819</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>23827</c:v>
+                  <c:v>2813565</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>3154692</c:v>
+                  <c:v>23892</c:v>
                 </c:pt>
                 <c:pt idx="26">
+                  <c:v>3160386</c:v>
+                </c:pt>
+                <c:pt idx="27">
                   <c:v>4043887</c:v>
                 </c:pt>
-                <c:pt idx="27">
-                  <c:v>1701121</c:v>
-                </c:pt>
                 <c:pt idx="28">
+                  <c:v>1704811</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>11840667</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>68469623</c:v>
+                </c:pt>
+                <c:pt idx="31">
                   <c:v>197339867</c:v>
                 </c:pt>
-                <c:pt idx="29">
-                  <c:v>251835</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>104175</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>187439</c:v>
-                </c:pt>
                 <c:pt idx="32">
-                  <c:v>297764</c:v>
+                  <c:v>251890</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>427340</c:v>
+                  <c:v>104182</c:v>
                 </c:pt>
                 <c:pt idx="34">
+                  <c:v>187551</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>374762287</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>297768</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>770382773</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>427342</c:v>
+                </c:pt>
+                <c:pt idx="39">
                   <c:v>8448281</c:v>
                 </c:pt>
-                <c:pt idx="35">
+                <c:pt idx="40">
                   <c:v>478450</c:v>
                 </c:pt>
-                <c:pt idx="36">
+                <c:pt idx="41">
                   <c:v>399856</c:v>
                 </c:pt>
-                <c:pt idx="37">
-                  <c:v>429391</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>13434107</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>820632</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>82242494</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>4612337</c:v>
-                </c:pt>
                 <c:pt idx="42">
-                  <c:v>840020</c:v>
+                  <c:v>503117290</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>2155897</c:v>
+                  <c:v>429409</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6532,20 +6620,21 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BEC4FA71-AAA7-E84F-A484-BC84FC126B46}">
-  <dimension ref="A1:F91"/>
+  <dimension ref="A1:F110"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="96" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:C91"/>
+      <selection activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="26.83203125" customWidth="1"/>
+    <col min="6" max="6" width="15.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -6559,12 +6648,12 @@
         <v>2</v>
       </c>
       <c r="D2" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B3">
         <v>18271</v>
@@ -6591,11 +6680,11 @@
         <v>1295</v>
       </c>
       <c r="C4">
-        <v>2392</v>
+        <v>2397</v>
       </c>
       <c r="D4" s="2">
         <f t="shared" ref="D4:D67" si="0">C4/B4</f>
-        <v>1.8471042471042471</v>
+        <v>1.850965250965251</v>
       </c>
       <c r="E4" s="1">
         <v>120000000</v>
@@ -6633,11 +6722,11 @@
         <v>127284</v>
       </c>
       <c r="C6">
-        <v>262327</v>
+        <v>262373</v>
       </c>
       <c r="D6" s="2">
         <f t="shared" si="0"/>
-        <v>2.0609581722761696</v>
+        <v>2.0613195688381887</v>
       </c>
       <c r="E6" s="1">
         <v>1200000</v>
@@ -6675,11 +6764,11 @@
         <v>359</v>
       </c>
       <c r="C8">
-        <v>549</v>
+        <v>554</v>
       </c>
       <c r="D8" s="2">
         <f t="shared" si="0"/>
-        <v>1.5292479108635098</v>
+        <v>1.5431754874651811</v>
       </c>
       <c r="E8" s="1">
         <v>1000000</v>
@@ -6726,11 +6815,11 @@
         <v>44178</v>
       </c>
       <c r="C11">
-        <v>81776</v>
+        <v>81780</v>
       </c>
       <c r="D11" s="2">
         <f t="shared" si="0"/>
-        <v>1.8510570872379917</v>
+        <v>1.8511476300421024</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
@@ -6741,11 +6830,11 @@
         <v>493</v>
       </c>
       <c r="C12">
-        <v>33206</v>
+        <v>33207</v>
       </c>
       <c r="D12" s="2">
         <f t="shared" si="0"/>
-        <v>67.354969574036517</v>
+        <v>67.356997971602439</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
@@ -6756,11 +6845,11 @@
         <v>605988</v>
       </c>
       <c r="C13">
-        <v>1117366</v>
+        <v>1117440</v>
       </c>
       <c r="D13" s="2">
         <f t="shared" si="0"/>
-        <v>1.8438747962005848</v>
+        <v>1.8439969108299175</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
@@ -6778,7 +6867,7 @@
         <v>3.3374982148630283</v>
       </c>
       <c r="E14" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
@@ -6789,18 +6878,18 @@
         <v>1197649</v>
       </c>
       <c r="C15">
-        <v>2211854</v>
+        <v>2211944</v>
       </c>
       <c r="D15" s="2">
         <f t="shared" si="0"/>
-        <v>1.8468299142737146</v>
+        <v>1.8469050614996547</v>
       </c>
       <c r="E15" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="F15" s="2">
         <f>MIN(D:D)</f>
-        <v>1.5292479108635098</v>
+        <v>1.5431754874651811</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
@@ -6818,11 +6907,11 @@
         <v>2.3906208481094851</v>
       </c>
       <c r="E16" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="F16" s="2">
         <f>MAX(D:D)</f>
-        <v>6072.9492957746479</v>
+        <v>6072.9577464788736</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
@@ -6840,11 +6929,11 @@
         <v>2.6640651510010178</v>
       </c>
       <c r="E17" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="F17" s="2">
         <f>AVERAGE(D:D)</f>
-        <v>117.65910878306588</v>
+        <v>112.86774897670921</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
@@ -6862,11 +6951,11 @@
         <v>2.6461630935684233</v>
       </c>
       <c r="E18" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="F18" s="2">
         <f>HARMEAN(D:D)</f>
-        <v>2.9314662896794688</v>
+        <v>3.1334336719081586</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
@@ -6877,11 +6966,11 @@
         <v>355617</v>
       </c>
       <c r="C19">
-        <v>721933</v>
+        <v>721935</v>
       </c>
       <c r="D19" s="2">
         <f t="shared" si="0"/>
-        <v>2.0300857383083484</v>
+        <v>2.0300913623364463</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
@@ -6913,6 +7002,9 @@
         <f t="shared" si="0"/>
         <v>2.1635833808205711</v>
       </c>
+      <c r="E21" t="s">
+        <v>124</v>
+      </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
@@ -6928,6 +7020,13 @@
         <f t="shared" si="0"/>
         <v>133.56231884057971</v>
       </c>
+      <c r="E22" t="s">
+        <v>125</v>
+      </c>
+      <c r="F22">
+        <f>MIN(B:B)</f>
+        <v>304</v>
+      </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
@@ -6937,11 +7036,18 @@
         <v>701346</v>
       </c>
       <c r="C23">
-        <v>1593572</v>
+        <v>1593947</v>
       </c>
       <c r="D23" s="2">
         <f t="shared" si="0"/>
-        <v>2.2721623848998926</v>
+        <v>2.2726970710605037</v>
+      </c>
+      <c r="E23" t="s">
+        <v>126</v>
+      </c>
+      <c r="F23">
+        <f>MAX(B:B)</f>
+        <v>325251378</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
@@ -6952,1016 +7058,1336 @@
         <v>3191</v>
       </c>
       <c r="C24">
-        <v>26361</v>
+        <v>26378</v>
       </c>
       <c r="D24" s="2">
         <f t="shared" si="0"/>
-        <v>8.2610466938263869</v>
+        <v>8.2663741773738639</v>
+      </c>
+      <c r="E24" t="s">
+        <v>127</v>
+      </c>
+      <c r="F24">
+        <f>AVERAGE(B:B)</f>
+        <v>14554539.546296297</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>19</v>
+        <v>98</v>
       </c>
       <c r="B25">
-        <v>467550</v>
+        <v>5985623</v>
       </c>
       <c r="C25">
-        <v>940813</v>
+        <v>28392373</v>
       </c>
       <c r="D25" s="2">
         <f t="shared" si="0"/>
-        <v>2.0122190140091969</v>
+        <v>4.7434282112321471</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>51</v>
+        <v>19</v>
       </c>
       <c r="B26">
-        <v>1318024</v>
+        <v>467550</v>
       </c>
       <c r="C26">
-        <v>2813556</v>
+        <v>940819</v>
       </c>
       <c r="D26" s="2">
         <f t="shared" si="0"/>
-        <v>2.1346773655107949</v>
+        <v>2.0122318468612983</v>
+      </c>
+      <c r="E26" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>20</v>
+        <v>51</v>
       </c>
       <c r="B27">
-        <v>4713</v>
+        <v>1318024</v>
       </c>
       <c r="C27">
-        <v>23827</v>
+        <v>2813565</v>
       </c>
       <c r="D27" s="2">
         <f t="shared" si="0"/>
-        <v>5.0555909187354127</v>
+        <v>2.1346841939145267</v>
+      </c>
+      <c r="E27" t="s">
+        <v>125</v>
+      </c>
+      <c r="F27" s="3">
+        <f>MIN(C:C)</f>
+        <v>554</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B28">
-        <v>1682059</v>
+        <v>4713</v>
       </c>
       <c r="C28">
-        <v>3154692</v>
+        <v>23892</v>
       </c>
       <c r="D28" s="2">
         <f t="shared" si="0"/>
-        <v>1.8754942603083482</v>
+        <v>5.0693825588796946</v>
+      </c>
+      <c r="E28" t="s">
+        <v>126</v>
+      </c>
+      <c r="F28" s="3">
+        <f>MAX(C:C)</f>
+        <v>770382773</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B29">
-        <v>1406192</v>
+        <v>1682059</v>
       </c>
       <c r="C29">
-        <v>4043887</v>
+        <v>3160386</v>
       </c>
       <c r="D29" s="2">
         <f t="shared" si="0"/>
-        <v>2.8757715873792482</v>
+        <v>1.8788793972149609</v>
+      </c>
+      <c r="E29" t="s">
+        <v>127</v>
+      </c>
+      <c r="F29" s="3">
+        <f>AVERAGE(C:C)</f>
+        <v>45001945.351851851</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B30">
-        <v>899701</v>
+        <v>1406192</v>
       </c>
       <c r="C30">
-        <v>1701121</v>
+        <v>4043887</v>
       </c>
       <c r="D30" s="2">
         <f t="shared" si="0"/>
-        <v>1.8907625977963791</v>
+        <v>2.8757715873792482</v>
+      </c>
+      <c r="F30" s="3">
+        <f>MEDIAN(C:C)</f>
+        <v>1719244.5</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>67</v>
+        <v>23</v>
       </c>
       <c r="B31">
-        <v>70651620</v>
+        <v>899701</v>
       </c>
       <c r="C31">
-        <v>197339867</v>
+        <v>1704811</v>
       </c>
       <c r="D31" s="2">
         <f t="shared" si="0"/>
-        <v>2.793140015756185</v>
+        <v>1.894863960360164</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>68</v>
+        <v>99</v>
       </c>
       <c r="B32">
-        <v>9567</v>
+        <v>4936014</v>
       </c>
       <c r="C32">
-        <v>251835</v>
+        <v>11840667</v>
       </c>
       <c r="D32" s="2">
         <f t="shared" si="0"/>
-        <v>26.32329883976168</v>
+        <v>2.3988317294075747</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>24</v>
+        <v>100</v>
       </c>
       <c r="B33">
-        <v>39501</v>
+        <v>8038928</v>
       </c>
       <c r="C33">
-        <v>104175</v>
+        <v>68469623</v>
       </c>
       <c r="D33" s="2">
         <f t="shared" si="0"/>
-        <v>2.6372750056960585</v>
+        <v>8.5172578980680012</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B34">
-        <v>18007</v>
+        <v>70651620</v>
       </c>
       <c r="C34">
-        <v>187439</v>
+        <v>197339867</v>
       </c>
       <c r="D34" s="2">
         <f t="shared" si="0"/>
-        <v>10.409229743988449</v>
+        <v>2.793140015756185</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>25</v>
+        <v>68</v>
       </c>
       <c r="B35">
-        <v>82194</v>
+        <v>9567</v>
       </c>
       <c r="C35">
-        <v>297764</v>
+        <v>251890</v>
       </c>
       <c r="D35" s="2">
         <f t="shared" si="0"/>
-        <v>3.6226975205002798</v>
+        <v>26.32904776837044</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>70</v>
+        <v>24</v>
       </c>
       <c r="B36">
-        <v>304</v>
+        <v>39501</v>
       </c>
       <c r="C36">
-        <v>427340</v>
+        <v>104182</v>
       </c>
       <c r="D36" s="2">
         <f t="shared" si="0"/>
-        <v>1405.7236842105262</v>
+        <v>2.6374522163995846</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>26</v>
+        <v>69</v>
       </c>
       <c r="B37">
-        <v>574062</v>
+        <v>18007</v>
       </c>
       <c r="C37">
-        <v>8448281</v>
+        <v>187551</v>
       </c>
       <c r="D37" s="2">
         <f t="shared" si="0"/>
-        <v>14.716669976413698</v>
+        <v>10.415449547398234</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>71</v>
+        <v>101</v>
       </c>
       <c r="B38">
-        <v>887</v>
+        <v>125319627</v>
       </c>
       <c r="C38">
-        <v>478450</v>
+        <v>374762287</v>
       </c>
       <c r="D38" s="2">
         <f t="shared" si="0"/>
-        <v>539.40248027057498</v>
+        <v>2.9904516632498437</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>72</v>
+        <v>25</v>
       </c>
       <c r="B39">
-        <v>1757</v>
+        <v>82194</v>
       </c>
       <c r="C39">
-        <v>399856</v>
+        <v>297768</v>
       </c>
       <c r="D39" s="2">
         <f t="shared" si="0"/>
-        <v>227.57882754695504</v>
+        <v>3.6227461858529821</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>54</v>
+        <v>102</v>
       </c>
       <c r="B40">
-        <v>190248</v>
+        <v>269645146</v>
       </c>
       <c r="C40">
-        <v>429391</v>
+        <v>770382773</v>
       </c>
       <c r="D40" s="2">
         <f t="shared" si="0"/>
-        <v>2.2570066439594636</v>
+        <v>2.8570244427837763</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>55</v>
+        <v>70</v>
       </c>
       <c r="B41">
-        <v>2064844</v>
+        <v>304</v>
       </c>
       <c r="C41">
-        <v>13434107</v>
+        <v>427342</v>
       </c>
       <c r="D41" s="2">
         <f t="shared" si="0"/>
-        <v>6.5061123261612019</v>
+        <v>1405.7302631578948</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>88</v>
+        <v>26</v>
       </c>
       <c r="B42">
-        <v>50722</v>
+        <v>574062</v>
       </c>
       <c r="C42">
-        <v>820632</v>
+        <v>8448281</v>
       </c>
       <c r="D42" s="2">
         <f t="shared" si="0"/>
-        <v>16.179015023066913</v>
+        <v>14.716669976413698</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>89</v>
+        <v>71</v>
       </c>
       <c r="B43">
-        <v>45923418</v>
+        <v>887</v>
       </c>
       <c r="C43">
-        <v>82242494</v>
+        <v>478450</v>
       </c>
       <c r="D43" s="2">
         <f t="shared" si="0"/>
-        <v>1.7908617777535636</v>
+        <v>539.40248027057498</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>90</v>
+        <v>72</v>
       </c>
       <c r="B44">
-        <v>72258</v>
+        <v>1757</v>
       </c>
       <c r="C44">
-        <v>4612337</v>
+        <v>399856</v>
       </c>
       <c r="D44" s="2">
         <f t="shared" si="0"/>
-        <v>63.831506545987985</v>
+        <v>227.57882754695504</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>47</v>
+        <v>103</v>
       </c>
       <c r="B45">
-        <v>401032</v>
+        <v>78873354</v>
       </c>
       <c r="C45">
-        <v>840020</v>
+        <v>503117290</v>
       </c>
       <c r="D45" s="2">
         <f t="shared" si="0"/>
-        <v>2.0946458138003949</v>
+        <v>6.3787992330084</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>91</v>
+        <v>54</v>
       </c>
       <c r="B46">
-        <v>355</v>
+        <v>190248</v>
       </c>
       <c r="C46">
-        <v>2155897</v>
+        <v>429409</v>
       </c>
       <c r="D46" s="2">
         <f t="shared" si="0"/>
-        <v>6072.9492957746479</v>
+        <v>2.2571012573062528</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="B47">
-        <v>1125105</v>
+        <v>2064844</v>
       </c>
       <c r="C47">
-        <v>4417763</v>
+        <v>13434107</v>
       </c>
       <c r="D47" s="2">
         <f t="shared" si="0"/>
-        <v>3.9265339679407698</v>
+        <v>6.5061123261612019</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>27</v>
+        <v>104</v>
       </c>
       <c r="B48">
-        <v>6074672</v>
+        <v>13737124</v>
       </c>
       <c r="C48">
-        <v>13104874</v>
+        <v>141587875</v>
       </c>
       <c r="D48" s="2">
         <f t="shared" si="0"/>
-        <v>2.1572973816528696</v>
+        <v>10.306951804467952</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>28</v>
+        <v>85</v>
       </c>
       <c r="B49">
-        <v>132891</v>
+        <v>50722</v>
       </c>
       <c r="C49">
-        <v>287927</v>
+        <v>820648</v>
       </c>
       <c r="D49" s="2">
         <f t="shared" si="0"/>
-        <v>2.1666403292924277</v>
+        <v>16.179330468041481</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>29</v>
+        <v>86</v>
       </c>
       <c r="B50">
-        <v>65522</v>
+        <v>45923418</v>
       </c>
       <c r="C50">
-        <v>136106</v>
+        <v>82243431</v>
       </c>
       <c r="D50" s="2">
         <f t="shared" si="0"/>
-        <v>2.0772564940020146</v>
+        <v>1.7908821812871158</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>56</v>
+        <v>105</v>
       </c>
       <c r="B51">
-        <v>15561156</v>
+        <v>83111464</v>
       </c>
       <c r="C51">
-        <v>38336161</v>
+        <v>188103550</v>
       </c>
       <c r="D51" s="2">
         <f t="shared" si="0"/>
-        <v>2.4635805334770757</v>
+        <v>2.2632683982079778</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>30</v>
+        <v>106</v>
       </c>
       <c r="B52">
-        <v>143191</v>
+        <v>40776253</v>
       </c>
       <c r="C52">
-        <v>298732</v>
+        <v>104351646</v>
       </c>
       <c r="D52" s="2">
         <f t="shared" si="0"/>
-        <v>2.086248437401792</v>
+        <v>2.5591278825938226</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>31</v>
+        <v>107</v>
       </c>
       <c r="B53">
-        <v>2851</v>
+        <v>79106742</v>
       </c>
       <c r="C53">
-        <v>7851</v>
+        <v>265990284</v>
       </c>
       <c r="D53" s="2">
         <f t="shared" si="0"/>
-        <v>2.7537706068046299</v>
+        <v>3.3624224342344928</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>32</v>
+        <v>108</v>
       </c>
       <c r="B54">
-        <v>5243</v>
+        <v>3133905</v>
       </c>
       <c r="C54">
-        <v>13911</v>
+        <v>23973053</v>
       </c>
       <c r="D54" s="2">
         <f t="shared" si="0"/>
-        <v>2.6532519549876024</v>
+        <v>7.6495787204781251</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>33</v>
+        <v>109</v>
       </c>
       <c r="B55">
-        <v>334862</v>
+        <v>16147</v>
       </c>
       <c r="C55">
-        <v>681295</v>
+        <v>1697847</v>
       </c>
       <c r="D55" s="2">
         <f t="shared" si="0"/>
-        <v>2.0345545329120651</v>
+        <v>105.149377593361</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>34</v>
+        <v>110</v>
       </c>
       <c r="B56">
-        <v>2659</v>
+        <v>45214</v>
       </c>
       <c r="C56">
-        <v>7335</v>
+        <v>1277037</v>
       </c>
       <c r="D56" s="2">
         <f t="shared" si="0"/>
-        <v>2.7585558480631818</v>
+        <v>28.244282744282746</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>35</v>
+        <v>87</v>
       </c>
       <c r="B57">
-        <v>82585</v>
+        <v>72258</v>
       </c>
       <c r="C57">
-        <v>317789</v>
+        <v>4612352</v>
       </c>
       <c r="D57" s="2">
         <f t="shared" si="0"/>
-        <v>3.8480232487739903</v>
+        <v>63.831714135459052</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>36</v>
+        <v>111</v>
       </c>
       <c r="B58">
-        <v>447979</v>
+        <v>905</v>
       </c>
       <c r="C58">
-        <v>1612224</v>
+        <v>2500003</v>
       </c>
       <c r="D58" s="2">
         <f t="shared" si="0"/>
-        <v>3.5988829833541303</v>
+        <v>2762.4342541436463</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>73</v>
+        <v>47</v>
       </c>
       <c r="B59">
-        <v>905899</v>
+        <v>401032</v>
       </c>
       <c r="C59">
-        <v>1733591</v>
+        <v>840020</v>
       </c>
       <c r="D59" s="2">
         <f t="shared" si="0"/>
-        <v>1.9136691838714912</v>
+        <v>2.0946458138003949</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>74</v>
+        <v>88</v>
       </c>
       <c r="B60">
-        <v>433226</v>
+        <v>355</v>
       </c>
       <c r="C60">
-        <v>802182</v>
+        <v>2155900</v>
       </c>
       <c r="D60" s="2">
         <f t="shared" si="0"/>
-        <v>1.8516478697031111</v>
+        <v>6072.9577464788736</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>75</v>
+        <v>112</v>
       </c>
       <c r="B61">
-        <v>551970</v>
+        <v>63050</v>
       </c>
       <c r="C61">
-        <v>1006230</v>
+        <v>4771522</v>
       </c>
       <c r="D61" s="2">
         <f t="shared" si="0"/>
-        <v>1.8229795097559649</v>
+        <v>75.678382236320374</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>37</v>
+        <v>113</v>
       </c>
       <c r="B62">
-        <v>1891045</v>
+        <v>3195277</v>
       </c>
       <c r="C62">
-        <v>3386906</v>
+        <v>6098685</v>
       </c>
       <c r="D62" s="2">
         <f t="shared" si="0"/>
-        <v>1.7910234817257125</v>
+        <v>1.9086561196415834</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>100</v>
+        <v>64</v>
       </c>
       <c r="B63">
-        <v>1210098</v>
+        <v>1125105</v>
       </c>
       <c r="C63">
-        <v>2232325</v>
+        <v>4417869</v>
       </c>
       <c r="D63" s="2">
         <f t="shared" si="0"/>
-        <v>1.8447472849306419</v>
+        <v>3.9266281813697388</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>57</v>
+        <v>114</v>
       </c>
       <c r="B64">
-        <v>1001050</v>
+        <v>325251378</v>
       </c>
       <c r="C64">
-        <v>2393131</v>
+        <v>736764776</v>
       </c>
       <c r="D64" s="2">
         <f t="shared" si="0"/>
-        <v>2.3906208481094851</v>
+        <v>2.2652164628184912</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>76</v>
+        <v>27</v>
       </c>
       <c r="B65">
-        <v>755273</v>
+        <v>6074672</v>
       </c>
       <c r="C65">
-        <v>1440860</v>
+        <v>13104909</v>
       </c>
       <c r="D65" s="2">
         <f t="shared" si="0"/>
-        <v>1.9077340246506893</v>
+        <v>2.1573031432808225</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="B66">
-        <v>470934</v>
+        <v>132891</v>
       </c>
       <c r="C66">
-        <v>1914084</v>
+        <v>287958</v>
       </c>
       <c r="D66" s="2">
         <f t="shared" si="0"/>
-        <v>4.0644421511294579</v>
+        <v>2.1668736031785447</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>77</v>
+        <v>29</v>
       </c>
       <c r="B67">
-        <v>1178453</v>
+        <v>65522</v>
       </c>
       <c r="C67">
-        <v>2188788</v>
+        <v>136116</v>
       </c>
       <c r="D67" s="2">
         <f t="shared" si="0"/>
-        <v>1.8573400890828908</v>
+        <v>2.0774091144958944</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>39</v>
+        <v>56</v>
       </c>
       <c r="B68">
-        <v>3131</v>
+        <v>15561156</v>
       </c>
       <c r="C68">
-        <v>8575</v>
+        <v>38336288</v>
       </c>
       <c r="D68" s="2">
-        <f t="shared" ref="D68:D91" si="1">C68/B68</f>
-        <v>2.7387416160970934</v>
+        <f t="shared" ref="D68:D110" si="1">C68/B68</f>
+        <v>2.4635886948244718</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="B69">
-        <v>2515</v>
+        <v>143191</v>
       </c>
       <c r="C69">
-        <v>6607</v>
+        <v>298755</v>
       </c>
       <c r="D69" s="2">
         <f t="shared" si="1"/>
-        <v>2.6270377733598411</v>
+        <v>2.0864090620220543</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>58</v>
+        <v>31</v>
       </c>
       <c r="B70">
-        <v>1903735</v>
+        <v>2851</v>
       </c>
       <c r="C70">
-        <v>4312279</v>
+        <v>7851</v>
       </c>
       <c r="D70" s="2">
         <f t="shared" si="1"/>
-        <v>2.2651676835273817</v>
+        <v>2.7537706068046299</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="B71">
-        <v>1107098</v>
+        <v>5243</v>
       </c>
       <c r="C71">
-        <v>1867578</v>
+        <v>13911</v>
       </c>
       <c r="D71" s="2">
         <f t="shared" si="1"/>
-        <v>1.6869129923457544</v>
+        <v>2.6532519549876024</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>78</v>
+        <v>33</v>
       </c>
       <c r="B72">
-        <v>1801878</v>
+        <v>334862</v>
       </c>
       <c r="C72">
-        <v>3324336</v>
+        <v>681444</v>
       </c>
       <c r="D72" s="2">
         <f t="shared" si="1"/>
-        <v>1.8449284579755123</v>
+        <v>2.0349994923281831</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>59</v>
+        <v>34</v>
       </c>
       <c r="B73">
-        <v>2437497</v>
+        <v>2659</v>
       </c>
       <c r="C73">
-        <v>5273728</v>
+        <v>7335</v>
       </c>
       <c r="D73" s="2">
         <f t="shared" si="1"/>
-        <v>2.1635833808205711</v>
+        <v>2.7585558480631818</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="B74">
-        <v>467550</v>
+        <v>82585</v>
       </c>
       <c r="C74">
-        <v>940813</v>
+        <v>317789</v>
       </c>
       <c r="D74" s="2">
         <f t="shared" si="1"/>
-        <v>2.0122190140091969</v>
+        <v>3.8480232487739903</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="B75">
-        <v>3109</v>
+        <v>447979</v>
       </c>
       <c r="C75">
-        <v>8227</v>
+        <v>1612224</v>
       </c>
       <c r="D75" s="2">
         <f t="shared" si="1"/>
-        <v>2.6461884850434223</v>
+        <v>3.5988829833541303</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>44</v>
+        <v>73</v>
       </c>
       <c r="B76">
-        <v>899701</v>
+        <v>905899</v>
       </c>
       <c r="C76">
-        <v>1701121</v>
+        <v>1733678</v>
       </c>
       <c r="D76" s="2">
         <f t="shared" si="1"/>
-        <v>1.8907625977963791</v>
+        <v>1.9137652210676908</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>60</v>
+        <v>74</v>
       </c>
       <c r="B77">
-        <v>312728</v>
+        <v>433226</v>
       </c>
       <c r="C77">
-        <v>642675</v>
+        <v>802268</v>
       </c>
       <c r="D77" s="2">
         <f t="shared" si="1"/>
-        <v>2.055060627765982</v>
+        <v>1.851846380411148</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="B78">
-        <v>18007</v>
+        <v>551970</v>
       </c>
       <c r="C78">
-        <v>187439</v>
+        <v>1006319</v>
       </c>
       <c r="D78" s="2">
         <f t="shared" si="1"/>
-        <v>10.409229743988449</v>
+        <v>1.8231407504031016</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>61</v>
+        <v>37</v>
       </c>
       <c r="B79">
-        <v>3175308</v>
+        <v>1891045</v>
       </c>
       <c r="C79">
-        <v>7838972</v>
+        <v>3387533</v>
       </c>
       <c r="D79" s="2">
         <f t="shared" si="1"/>
-        <v>2.4687280729932342</v>
+        <v>1.7913550444331043</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>80</v>
+        <v>97</v>
       </c>
       <c r="B80">
-        <v>142059</v>
+        <v>1210098</v>
       </c>
       <c r="C80">
-        <v>747752</v>
+        <v>2232426</v>
       </c>
       <c r="D80" s="2">
         <f t="shared" si="1"/>
-        <v>5.2636721362250896</v>
+        <v>1.8448307492451024</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>45</v>
+        <v>76</v>
       </c>
       <c r="B81">
-        <v>453769</v>
+        <v>755273</v>
       </c>
       <c r="C81">
-        <v>1563727</v>
+        <v>1440924</v>
       </c>
       <c r="D81" s="2">
         <f t="shared" si="1"/>
-        <v>3.4460860041122245</v>
+        <v>1.9078187622224017</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>62</v>
+        <v>38</v>
       </c>
       <c r="B82">
-        <v>498246</v>
+        <v>470934</v>
       </c>
       <c r="C82">
-        <v>1154507</v>
+        <v>1914084</v>
       </c>
       <c r="D82" s="2">
         <f t="shared" si="1"/>
-        <v>2.3171425360163451</v>
+        <v>4.0644421511294579</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="B83">
-        <v>304</v>
+        <v>1178453</v>
       </c>
       <c r="C83">
-        <v>427340</v>
+        <v>2188886</v>
       </c>
       <c r="D83" s="2">
         <f t="shared" si="1"/>
-        <v>1405.7236842105262</v>
+        <v>1.8574232489543494</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>82</v>
+        <v>39</v>
       </c>
       <c r="B84">
-        <v>797866</v>
+        <v>3131</v>
       </c>
       <c r="C84">
-        <v>6840229</v>
+        <v>8575</v>
       </c>
       <c r="D84" s="2">
         <f t="shared" si="1"/>
-        <v>8.5731551413395231</v>
+        <v>2.7387416160970934</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>63</v>
+        <v>40</v>
       </c>
       <c r="B85">
-        <v>3835114</v>
+        <v>2515</v>
       </c>
       <c r="C85">
-        <v>17412807</v>
+        <v>6607</v>
       </c>
       <c r="D85" s="2">
         <f t="shared" si="1"/>
-        <v>4.5403622943151101</v>
+        <v>2.6270377733598411</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>83</v>
+        <v>58</v>
       </c>
       <c r="B86">
-        <v>50722</v>
+        <v>1903735</v>
       </c>
       <c r="C86">
-        <v>820632</v>
+        <v>4312279</v>
       </c>
       <c r="D86" s="2">
         <f t="shared" si="1"/>
-        <v>16.179015023066913</v>
+        <v>2.2651676835273817</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>84</v>
+        <v>41</v>
       </c>
       <c r="B87">
-        <v>647011</v>
+        <v>1107098</v>
       </c>
       <c r="C87">
-        <v>9905335</v>
+        <v>1868005</v>
       </c>
       <c r="D87" s="2">
         <f t="shared" si="1"/>
-        <v>15.309376502099655</v>
+        <v>1.6872986853918985</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="B88">
-        <v>5189</v>
+        <v>1801878</v>
       </c>
       <c r="C88">
-        <v>1234643</v>
+        <v>3324418</v>
       </c>
       <c r="D88" s="2">
         <f t="shared" si="1"/>
-        <v>237.93466949315859</v>
+        <v>1.8449739660509756</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>86</v>
+        <v>115</v>
       </c>
       <c r="B89">
-        <v>740235</v>
+        <v>47556240</v>
       </c>
       <c r="C89">
-        <v>2672407</v>
+        <v>206213289</v>
       </c>
       <c r="D89" s="2">
         <f t="shared" si="1"/>
-        <v>3.6102143238295947</v>
+        <v>4.3361983411640619</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>46</v>
+        <v>116</v>
       </c>
       <c r="B90">
-        <v>402460</v>
+        <v>24087642</v>
       </c>
       <c r="C90">
-        <v>844395</v>
+        <v>83491057</v>
       </c>
       <c r="D90" s="2">
         <f t="shared" si="1"/>
-        <v>2.0980842816677434</v>
+        <v>3.4661365774200728</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>87</v>
+        <v>43</v>
       </c>
       <c r="B91">
-        <v>3975194</v>
+        <v>3109</v>
       </c>
       <c r="C91">
-        <v>16763034</v>
+        <v>8227</v>
       </c>
       <c r="D91" s="2">
         <f t="shared" si="1"/>
-        <v>4.2169096652892915</v>
+        <v>2.6461884850434223</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A92" t="s">
+        <v>117</v>
+      </c>
+      <c r="B92">
+        <v>16038150</v>
+      </c>
+      <c r="C92">
+        <v>101261480</v>
+      </c>
+      <c r="D92" s="2">
+        <f t="shared" si="1"/>
+        <v>6.3137880615906452</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A93" t="s">
+        <v>60</v>
+      </c>
+      <c r="B93">
+        <v>312728</v>
+      </c>
+      <c r="C93">
+        <v>642675</v>
+      </c>
+      <c r="D93" s="2">
+        <f t="shared" si="1"/>
+        <v>2.055060627765982</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A94" t="s">
+        <v>61</v>
+      </c>
+      <c r="B94">
+        <v>3175308</v>
+      </c>
+      <c r="C94">
+        <v>7847036</v>
+      </c>
+      <c r="D94" s="2">
+        <f t="shared" si="1"/>
+        <v>2.4712676691520947</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A95" t="s">
+        <v>79</v>
+      </c>
+      <c r="B95">
+        <v>142059</v>
+      </c>
+      <c r="C95">
+        <v>747752</v>
+      </c>
+      <c r="D95" s="2">
+        <f t="shared" si="1"/>
+        <v>5.2636721362250896</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A96" t="s">
+        <v>118</v>
+      </c>
+      <c r="B96">
+        <v>20382514</v>
+      </c>
+      <c r="C96">
+        <v>69650789</v>
+      </c>
+      <c r="D96" s="2">
+        <f t="shared" si="1"/>
+        <v>3.4171834249690689</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A97" t="s">
+        <v>45</v>
+      </c>
+      <c r="B97">
+        <v>453769</v>
+      </c>
+      <c r="C97">
+        <v>1563728</v>
+      </c>
+      <c r="D97" s="2">
+        <f t="shared" si="1"/>
+        <v>3.446088207876695</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A98" t="s">
+        <v>62</v>
+      </c>
+      <c r="B98">
+        <v>498246</v>
+      </c>
+      <c r="C98">
+        <v>1154507</v>
+      </c>
+      <c r="D98" s="2">
+        <f t="shared" si="1"/>
+        <v>2.3171425360163451</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A99" t="s">
+        <v>80</v>
+      </c>
+      <c r="B99">
+        <v>797866</v>
+      </c>
+      <c r="C99">
+        <v>6840229</v>
+      </c>
+      <c r="D99" s="2">
+        <f t="shared" si="1"/>
+        <v>8.5731551413395231</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A100" t="s">
+        <v>63</v>
+      </c>
+      <c r="B100">
+        <v>3835114</v>
+      </c>
+      <c r="C100">
+        <v>17412807</v>
+      </c>
+      <c r="D100" s="2">
+        <f t="shared" si="1"/>
+        <v>4.5403622943151101</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A101" t="s">
+        <v>119</v>
+      </c>
+      <c r="B101">
+        <v>5035130</v>
+      </c>
+      <c r="C101">
+        <v>10668725</v>
+      </c>
+      <c r="D101" s="2">
+        <f t="shared" si="1"/>
+        <v>2.1188579043639391</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A102" t="s">
+        <v>81</v>
+      </c>
+      <c r="B102">
+        <v>647011</v>
+      </c>
+      <c r="C102">
+        <v>9905453</v>
+      </c>
+      <c r="D102" s="2">
+        <f t="shared" si="1"/>
+        <v>15.309558879215345</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A103" t="s">
+        <v>82</v>
+      </c>
+      <c r="B103">
+        <v>5189</v>
+      </c>
+      <c r="C103">
+        <v>1234644</v>
+      </c>
+      <c r="D103" s="2">
+        <f t="shared" si="1"/>
+        <v>237.93486220851801</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A104" t="s">
+        <v>83</v>
+      </c>
+      <c r="B104">
+        <v>740235</v>
+      </c>
+      <c r="C104">
+        <v>2672407</v>
+      </c>
+      <c r="D104" s="2">
+        <f t="shared" si="1"/>
+        <v>3.6102143238295947</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A105" t="s">
+        <v>120</v>
+      </c>
+      <c r="B105">
+        <v>219979530</v>
+      </c>
+      <c r="C105">
+        <v>417455256</v>
+      </c>
+      <c r="D105" s="2">
+        <f t="shared" si="1"/>
+        <v>1.8977004633112908</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A106" t="s">
+        <v>46</v>
+      </c>
+      <c r="B106">
+        <v>402460</v>
+      </c>
+      <c r="C106">
+        <v>844395</v>
+      </c>
+      <c r="D106" s="2">
+        <f t="shared" si="1"/>
+        <v>2.0980842816677434</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A107" t="s">
+        <v>121</v>
+      </c>
+      <c r="B107">
+        <v>2295530</v>
+      </c>
+      <c r="C107">
+        <v>81147729</v>
+      </c>
+      <c r="D107" s="2">
+        <f t="shared" si="1"/>
+        <v>35.350323890343404</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A108" t="s">
+        <v>122</v>
+      </c>
+      <c r="B108">
+        <v>1772352</v>
+      </c>
+      <c r="C108">
+        <v>119113610</v>
+      </c>
+      <c r="D108" s="2">
+        <f t="shared" si="1"/>
+        <v>67.206519923807463</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A109" t="s">
+        <v>84</v>
+      </c>
+      <c r="B109">
+        <v>3975194</v>
+      </c>
+      <c r="C109">
+        <v>16763326</v>
+      </c>
+      <c r="D109" s="2">
+        <f t="shared" si="1"/>
+        <v>4.2169831208237891</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A110" t="s">
+        <v>123</v>
+      </c>
+      <c r="B110">
+        <v>8493275</v>
+      </c>
+      <c r="C110">
+        <v>41873955</v>
+      </c>
+      <c r="D110" s="2">
+        <f t="shared" si="1"/>
+        <v>4.9302483435423907</v>
       </c>
     </row>
   </sheetData>

</xml_diff>